<commit_message>
Datasets resultantes e integrados con barrios
</commit_message>
<xml_diff>
--- a/data_preprocesada_N1/desempleados_población_2016.xlsx
+++ b/data_preprocesada_N1/desempleados_población_2016.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="161">
   <si>
     <t>INDICADOR</t>
   </si>
@@ -28,6 +28,12 @@
     <t>ANIO</t>
   </si>
   <si>
+    <t>LATITUD</t>
+  </si>
+  <si>
+    <t>LONGITUD</t>
+  </si>
+  <si>
     <t>Número de Parados (Junio 2016)</t>
   </si>
   <si>
@@ -79,7 +85,7 @@
     <t>RETIRO</t>
   </si>
   <si>
-    <t>PACIFICO</t>
+    <t>PACÍFICO</t>
   </si>
   <si>
     <t>ADELFAS</t>
@@ -154,7 +160,7 @@
     <t>ALMENARA</t>
   </si>
   <si>
-    <t>VALDEACEREDAS</t>
+    <t>VALDEACEDERAS</t>
   </si>
   <si>
     <t>BERRUGUETE</t>
@@ -175,7 +181,7 @@
     <t>ALMAGRO</t>
   </si>
   <si>
-    <t>RIOS ROSAS</t>
+    <t>RÍOS ROSAS</t>
   </si>
   <si>
     <t>VALLEHERMOSO</t>
@@ -188,13 +194,13 @@
     <t>EL PARDO</t>
   </si>
   <si>
-    <t>FUENTELARREINA</t>
+    <t>FUENTELAREINA</t>
   </si>
   <si>
     <t>PEÑAGRANDE</t>
   </si>
   <si>
-    <t>EL PILAR</t>
+    <t>PILAR</t>
   </si>
   <si>
     <t>LA PAZ</t>
@@ -219,8 +225,7 @@
     <t>ARGÜELLES</t>
   </si>
   <si>
-    <t>CIUDAD 
-UNIVERSITARIA</t>
+    <t>CIUDAD UNIVERSITARIA</t>
   </si>
   <si>
     <t>VALDEZARZA</t>
@@ -320,8 +325,7 @@
     <t>PALOMERAS BAJAS</t>
   </si>
   <si>
-    <t>PALOMERAS 
-SURESTE</t>
+    <t>PALOMERAS SURESTE</t>
   </si>
   <si>
     <t>PORTAZGO</t>
@@ -354,7 +358,7 @@
     <t>CIUDAD LINEAL</t>
   </si>
   <si>
-    <t xml:space="preserve">VENTAS </t>
+    <t>VENTAS</t>
   </si>
   <si>
     <t>PUEBLO NUEVO</t>
@@ -369,8 +373,7 @@
     <t>SAN PASCUAL</t>
   </si>
   <si>
-    <t>SAN JUAN 
-BAUTISTA</t>
+    <t>SAN JUAN BAUTISTA</t>
   </si>
   <si>
     <t>COLINA</t>
@@ -397,7 +400,7 @@
     <t>PINAR DEL REY</t>
   </si>
   <si>
-    <t>APÓSTOLO SANTIAGO</t>
+    <t>APÓSTOL SANTIAGO</t>
   </si>
   <si>
     <t>VALDEFUENTES</t>
@@ -431,8 +434,7 @@
  VALLECAS</t>
   </si>
   <si>
-    <t>CASCO HISTÓRICO DE
-VALLECAS</t>
+    <t>CASCO HISTÓRICO DE VALLECAS</t>
   </si>
   <si>
     <t>SANTA EUGENIA</t>
@@ -450,8 +452,7 @@
     <t>VICÁLVARO</t>
   </si>
   <si>
-    <t>CASCO HISTÓRICO DE
-VICÁLVARO</t>
+    <t>CASCO HISTÓRICO DE VICÁLVARO</t>
   </si>
   <si>
     <t>AMBROZ</t>
@@ -494,11 +495,10 @@
     <t>AEROPUERTO</t>
   </si>
   <si>
-    <t>CASCO HISTÓRICO
-DE BARAJAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIMÓN </t>
+    <t>CASCO HISTÓRICO DE BARAJAS</t>
+  </si>
+  <si>
+    <t>TIMÓN</t>
   </si>
   <si>
     <t>CORRALEJOS</t>
@@ -859,13 +859,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,16 +878,22 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>9008</v>
@@ -896,15 +902,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>1362</v>
@@ -912,16 +918,22 @@
       <c r="E3">
         <v>2016</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>4474110.875</v>
+      </c>
+      <c r="G3">
+        <v>439417.7914</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>3349</v>
@@ -929,16 +941,22 @@
       <c r="E4">
         <v>2016</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>4473417.211</v>
+      </c>
+      <c r="G4">
+        <v>440397.1764</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>672</v>
@@ -946,16 +964,22 @@
       <c r="E5">
         <v>2016</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>4474035.577</v>
+      </c>
+      <c r="G5">
+        <v>440880.1521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>875</v>
@@ -963,16 +987,22 @@
       <c r="E6">
         <v>2016</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>4475014.208</v>
+      </c>
+      <c r="G6">
+        <v>440900.7625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>1856</v>
@@ -980,16 +1010,22 @@
       <c r="E7">
         <v>2016</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>4475244.247</v>
+      </c>
+      <c r="G7">
+        <v>440020.8477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>471</v>
@@ -997,16 +1033,22 @@
       <c r="E8">
         <v>2016</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>4474314.564</v>
+      </c>
+      <c r="G8">
+        <v>440226.8442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>8290</v>
@@ -1015,15 +1057,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>1169</v>
@@ -1031,16 +1073,22 @@
       <c r="E10">
         <v>2016</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>4473089.616</v>
+      </c>
+      <c r="G10">
+        <v>439045.6199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>1803</v>
@@ -1048,16 +1096,22 @@
       <c r="E11">
         <v>2016</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>4472513.434</v>
+      </c>
+      <c r="G11">
+        <v>439982.8536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>1274</v>
@@ -1065,16 +1119,22 @@
       <c r="E12">
         <v>2016</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>4471808.825</v>
+      </c>
+      <c r="G12">
+        <v>440672.2536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>755</v>
@@ -1082,16 +1142,22 @@
       <c r="E13">
         <v>2016</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>4471151.447</v>
+      </c>
+      <c r="G13">
+        <v>441682.9396</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>1384</v>
@@ -1099,16 +1165,22 @@
       <c r="E14">
         <v>2016</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>4472027.934</v>
+      </c>
+      <c r="G14">
+        <v>441453.464</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>1517</v>
@@ -1116,16 +1188,22 @@
       <c r="E15">
         <v>2016</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>4472774.286</v>
+      </c>
+      <c r="G15">
+        <v>441057.6445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <v>64</v>
@@ -1133,16 +1211,22 @@
       <c r="E16">
         <v>2016</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>4472353.007</v>
+      </c>
+      <c r="G16">
+        <v>442131.2346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <v>4788</v>
@@ -1151,15 +1235,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <v>1478</v>
@@ -1167,16 +1251,22 @@
       <c r="E18">
         <v>2016</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>4472859.079</v>
+      </c>
+      <c r="G18">
+        <v>442407.5013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19">
         <v>878</v>
@@ -1184,16 +1274,22 @@
       <c r="E19">
         <v>2016</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>4472494.747</v>
+      </c>
+      <c r="G19">
+        <v>443062.2345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D20">
         <v>729</v>
@@ -1201,16 +1297,22 @@
       <c r="E20">
         <v>2016</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <v>4473931.01</v>
+      </c>
+      <c r="G20">
+        <v>443534.9304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21">
         <v>851</v>
@@ -1218,16 +1320,22 @@
       <c r="E21">
         <v>2016</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>4474469.277</v>
+      </c>
+      <c r="G21">
+        <v>442791.7959</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D22">
         <v>201</v>
@@ -1235,16 +1343,22 @@
       <c r="E22">
         <v>2016</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <v>4473905.687</v>
+      </c>
+      <c r="G22">
+        <v>441870.6698</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D23">
         <v>433</v>
@@ -1252,16 +1366,22 @@
       <c r="E23">
         <v>2016</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>4473660.907</v>
+      </c>
+      <c r="G23">
+        <v>442862.905</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D24">
         <v>5717</v>
@@ -1270,15 +1390,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D25">
         <v>430</v>
@@ -1286,16 +1406,22 @@
       <c r="E25">
         <v>2016</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>4475110.43</v>
+      </c>
+      <c r="G25">
+        <v>441820.8979</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D26">
         <v>1106</v>
@@ -1303,16 +1429,22 @@
       <c r="E26">
         <v>2016</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>4475153.753</v>
+      </c>
+      <c r="G26">
+        <v>442789.9119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D27">
         <v>989</v>
@@ -1320,16 +1452,22 @@
       <c r="E27">
         <v>2016</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>4475116.489</v>
+      </c>
+      <c r="G27">
+        <v>443691.2602</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D28">
         <v>1712</v>
@@ -1337,16 +1475,22 @@
       <c r="E28">
         <v>2016</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>4476402.061</v>
+      </c>
+      <c r="G28">
+        <v>443463.5845</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D29">
         <v>772</v>
@@ -1354,16 +1498,22 @@
       <c r="E29">
         <v>2016</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>4475927.641</v>
+      </c>
+      <c r="G29">
+        <v>442676.6687</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D30">
         <v>432</v>
@@ -1371,16 +1521,22 @@
       <c r="E30">
         <v>2016</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>4476104.298</v>
+      </c>
+      <c r="G30">
+        <v>441959.5528</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D31">
         <v>5526</v>
@@ -1389,15 +1545,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>407</v>
@@ -1405,16 +1561,22 @@
       <c r="E32">
         <v>2016</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>4477360.964</v>
+      </c>
+      <c r="G32">
+        <v>441927.2958</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D33">
         <v>1800</v>
@@ -1422,16 +1584,22 @@
       <c r="E33">
         <v>2016</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>4477279.652</v>
+      </c>
+      <c r="G33">
+        <v>443241.5164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D34">
         <v>909</v>
@@ -1439,16 +1607,22 @@
       <c r="E34">
         <v>2016</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>4477733.182</v>
+      </c>
+      <c r="G34">
+        <v>442929.7851</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D35">
         <v>978</v>
@@ -1456,16 +1630,22 @@
       <c r="E35">
         <v>2016</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>4478520.651</v>
+      </c>
+      <c r="G35">
+        <v>442584.7337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D36">
         <v>679</v>
@@ -1473,16 +1653,22 @@
       <c r="E36">
         <v>2016</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>4479342.236</v>
+      </c>
+      <c r="G36">
+        <v>442506.6745</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D37">
         <v>584</v>
@@ -1490,16 +1676,22 @@
       <c r="E37">
         <v>2016</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>4480625.699</v>
+      </c>
+      <c r="G37">
+        <v>442382.2751</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D38">
         <v>9777</v>
@@ -1508,15 +1700,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D39">
         <v>1838</v>
@@ -1524,16 +1716,22 @@
       <c r="E39">
         <v>2016</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>4478217.699</v>
+      </c>
+      <c r="G39">
+        <v>439996.5425</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D40">
         <v>1601</v>
@@ -1541,16 +1739,22 @@
       <c r="E40">
         <v>2016</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <v>4478108.124</v>
+      </c>
+      <c r="G40">
+        <v>440893.969</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D41">
         <v>902</v>
@@ -1558,16 +1762,22 @@
       <c r="E41">
         <v>2016</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <v>4479092.74</v>
+      </c>
+      <c r="G41">
+        <v>441146.7116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D42">
         <v>1832</v>
@@ -1575,16 +1785,22 @@
       <c r="E42">
         <v>2016</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <v>4480229.372</v>
+      </c>
+      <c r="G42">
+        <v>441142.6001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D43">
         <v>1746</v>
@@ -1592,16 +1808,22 @@
       <c r="E43">
         <v>2016</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <v>4479832.029</v>
+      </c>
+      <c r="G43">
+        <v>440304.6074</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D44">
         <v>1595</v>
@@ -1609,16 +1831,22 @@
       <c r="E44">
         <v>2016</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <v>4479011.421</v>
+      </c>
+      <c r="G44">
+        <v>440230.3974</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D45">
         <v>5743</v>
@@ -1627,15 +1855,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D46">
         <v>993</v>
@@ -1643,16 +1871,22 @@
       <c r="E46">
         <v>2016</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <v>4476283.322</v>
+      </c>
+      <c r="G46">
+        <v>439389.8945</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D47">
         <v>974</v>
@@ -1660,16 +1894,22 @@
       <c r="E47">
         <v>2016</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <v>4476214.595</v>
+      </c>
+      <c r="G47">
+        <v>439947.5584</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D48">
         <v>1097</v>
@@ -1677,16 +1917,22 @@
       <c r="E48">
         <v>2016</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <v>4476037.29</v>
+      </c>
+      <c r="G48">
+        <v>440530.8517</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D49">
         <v>608</v>
@@ -1694,16 +1940,22 @@
       <c r="E49">
         <v>2016</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <v>4476032.059</v>
+      </c>
+      <c r="G49">
+        <v>441174.9953</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D50">
         <v>1000</v>
@@ -1711,16 +1963,22 @@
       <c r="E50">
         <v>2016</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <v>4477096.745</v>
+      </c>
+      <c r="G50">
+        <v>440826.6665</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D51">
         <v>620</v>
@@ -1728,16 +1986,22 @@
       <c r="E51">
         <v>2016</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <v>4477158.887</v>
+      </c>
+      <c r="G51">
+        <v>439682.3814</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D52">
         <v>10621</v>
@@ -1746,15 +2010,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D53">
         <v>149</v>
@@ -1762,16 +2026,22 @@
       <c r="E53">
         <v>2016</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <v>4489409.578</v>
+      </c>
+      <c r="G53">
+        <v>435018.7103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D54">
         <v>82</v>
@@ -1779,16 +2049,22 @@
       <c r="E54">
         <v>2016</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <v>4481421.762</v>
+      </c>
+      <c r="G54">
+        <v>437127.6497</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D55">
         <v>2157</v>
@@ -1796,16 +2072,22 @@
       <c r="E55">
         <v>2016</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <v>4481152.656</v>
+      </c>
+      <c r="G55">
+        <v>438480.3153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D56">
         <v>2413</v>
@@ -1813,16 +2095,22 @@
       <c r="E56">
         <v>2016</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <v>4480959.021</v>
+      </c>
+      <c r="G56">
+        <v>439853.0231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D57">
         <v>1199</v>
@@ -1830,16 +2118,22 @@
       <c r="E57">
         <v>2016</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <v>4481394.724</v>
+      </c>
+      <c r="G57">
+        <v>440957.8603</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D58">
         <v>3023</v>
@@ -1847,16 +2141,22 @@
       <c r="E58">
         <v>2016</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <v>4483501.173</v>
+      </c>
+      <c r="G58">
+        <v>442483.6118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D59">
         <v>898</v>
@@ -1864,16 +2164,22 @@
       <c r="E59">
         <v>2016</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <v>4483094.181</v>
+      </c>
+      <c r="G59">
+        <v>439024.2924</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D60">
         <v>462</v>
@@ -1881,16 +2187,22 @@
       <c r="E60">
         <v>2016</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <v>4487307.227</v>
+      </c>
+      <c r="G60">
+        <v>440716.0024</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D61">
         <v>4825</v>
@@ -1899,15 +2211,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D62">
         <v>635</v>
@@ -1915,16 +2227,22 @@
       <c r="E62">
         <v>2016</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <v>4475050.323</v>
+      </c>
+      <c r="G62">
+        <v>436118.4975</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D63">
         <v>930</v>
@@ -1932,16 +2250,22 @@
       <c r="E63">
         <v>2016</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <v>4475533.294</v>
+      </c>
+      <c r="G63">
+        <v>439109.0847</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D64">
         <v>500</v>
@@ -1949,16 +2273,22 @@
       <c r="E64">
         <v>2016</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64">
+        <v>4478627.02</v>
+      </c>
+      <c r="G64">
+        <v>437391.5065</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D65">
         <v>1606</v>
@@ -1966,16 +2296,22 @@
       <c r="E65">
         <v>2016</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65">
+        <v>4479644.899</v>
+      </c>
+      <c r="G65">
+        <v>439188.6628</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="1">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D66">
         <v>125</v>
@@ -1983,16 +2319,22 @@
       <c r="E66">
         <v>2016</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66">
+        <v>4480009.063</v>
+      </c>
+      <c r="G66">
+        <v>433968.0416</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="1">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D67">
         <v>58</v>
@@ -2000,16 +2342,22 @@
       <c r="E67">
         <v>2016</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67">
+        <v>4480219.592</v>
+      </c>
+      <c r="G67">
+        <v>430409.7127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="1">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D68">
         <v>738</v>
@@ -2017,16 +2365,22 @@
       <c r="E68">
         <v>2016</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68">
+        <v>4478516.428</v>
+      </c>
+      <c r="G68">
+        <v>433939.3352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="1">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D69">
         <v>15920</v>
@@ -2035,15 +2389,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:7">
       <c r="A70" s="1">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D70">
         <v>1432</v>
@@ -2051,16 +2405,22 @@
       <c r="E70">
         <v>2016</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70">
+        <v>4472579.69</v>
+      </c>
+      <c r="G70">
+        <v>437550.3787</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="1">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D71">
         <v>3089</v>
@@ -2068,16 +2428,22 @@
       <c r="E71">
         <v>2016</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71">
+        <v>4473487.258</v>
+      </c>
+      <c r="G71">
+        <v>437907.9825</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="1">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D72">
         <v>2534</v>
@@ -2085,16 +2451,22 @@
       <c r="E72">
         <v>2016</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72">
+        <v>4472679.645</v>
+      </c>
+      <c r="G72">
+        <v>436327.8871</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="1">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D73">
         <v>3944</v>
@@ -2102,16 +2474,22 @@
       <c r="E73">
         <v>2016</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73">
+        <v>4471531.816</v>
+      </c>
+      <c r="G73">
+        <v>435779.5365</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="1">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D74">
         <v>1156</v>
@@ -2119,16 +2497,22 @@
       <c r="E74">
         <v>2016</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74">
+        <v>4470817.836</v>
+      </c>
+      <c r="G74">
+        <v>431786.0869</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="1">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D75">
         <v>325</v>
@@ -2136,16 +2520,22 @@
       <c r="E75">
         <v>2016</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75">
+        <v>4468973.502</v>
+      </c>
+      <c r="G75">
+        <v>433434.5775</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="1">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D76">
         <v>3079</v>
@@ -2153,16 +2543,22 @@
       <c r="E76">
         <v>2016</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76">
+        <v>4470420.122</v>
+      </c>
+      <c r="G76">
+        <v>434547.9376</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="1">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D77">
         <v>18802</v>
@@ -2171,15 +2567,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:7">
       <c r="A78" s="1">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D78">
         <v>1597</v>
@@ -2187,16 +2583,22 @@
       <c r="E78">
         <v>2016</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78">
+        <v>4471676.723</v>
+      </c>
+      <c r="G78">
+        <v>439576.9792</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="1">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D79">
         <v>2282</v>
@@ -2204,16 +2606,22 @@
       <c r="E79">
         <v>2016</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79">
+        <v>4471320.131</v>
+      </c>
+      <c r="G79">
+        <v>438741.1131</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="1">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D80">
         <v>3401</v>
@@ -2221,16 +2629,22 @@
       <c r="E80">
         <v>2016</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80">
+        <v>4472031.606</v>
+      </c>
+      <c r="G80">
+        <v>438190.5428</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D81">
         <v>3329</v>
@@ -2238,16 +2652,22 @@
       <c r="E81">
         <v>2016</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81">
+        <v>4470681.208</v>
+      </c>
+      <c r="G81">
+        <v>436700.7182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="1">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D82">
         <v>2703</v>
@@ -2255,16 +2675,22 @@
       <c r="E82">
         <v>2016</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82">
+        <v>4470159.472</v>
+      </c>
+      <c r="G82">
+        <v>437262.2706</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="1">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D83">
         <v>2909</v>
@@ -2272,16 +2698,22 @@
       <c r="E83">
         <v>2016</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83">
+        <v>4468769.588</v>
+      </c>
+      <c r="G83">
+        <v>436656.9012</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="1">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D84">
         <v>2218</v>
@@ -2289,16 +2721,22 @@
       <c r="E84">
         <v>2016</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84">
+        <v>4470074.329</v>
+      </c>
+      <c r="G84">
+        <v>438358.4198</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="1">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D85">
         <v>10840</v>
@@ -2307,15 +2745,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:7">
       <c r="A86" s="1">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D86">
         <v>1742</v>
@@ -2323,16 +2761,22 @@
       <c r="E86">
         <v>2016</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <v>4468916.31</v>
+      </c>
+      <c r="G86">
+        <v>439516.2653</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="1">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D87">
         <v>1288</v>
@@ -2340,16 +2784,22 @@
       <c r="E87">
         <v>2016</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <v>4469305.319</v>
+      </c>
+      <c r="G87">
+        <v>440733.1193</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="1">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D88">
         <v>1909</v>
@@ -2357,16 +2807,22 @@
       <c r="E88">
         <v>2016</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <v>4469120.886</v>
+      </c>
+      <c r="G88">
+        <v>441499.985</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="1">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D89">
         <v>1562</v>
@@ -2374,16 +2830,22 @@
       <c r="E89">
         <v>2016</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89">
+        <v>4470576.407</v>
+      </c>
+      <c r="G89">
+        <v>440645.9665</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="1">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C90" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D90">
         <v>1844</v>
@@ -2391,16 +2853,22 @@
       <c r="E90">
         <v>2016</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90">
+        <v>4471173.407</v>
+      </c>
+      <c r="G90">
+        <v>440009.8419</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="1">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D91">
         <v>1124</v>
@@ -2408,16 +2876,22 @@
       <c r="E91">
         <v>2016</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91">
+        <v>4470110.376</v>
+      </c>
+      <c r="G91">
+        <v>439279.8576</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="1">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D92">
         <v>1238</v>
@@ -2425,16 +2899,22 @@
       <c r="E92">
         <v>2016</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92">
+        <v>4469968.652</v>
+      </c>
+      <c r="G92">
+        <v>439974.4688</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="1">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D93">
         <v>21403</v>
@@ -2443,15 +2923,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:7">
       <c r="A94" s="1">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D94">
         <v>3434</v>
@@ -2459,16 +2939,22 @@
       <c r="E94">
         <v>2016</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94">
+        <v>4469574.278</v>
+      </c>
+      <c r="G94">
+        <v>442858.5724</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="1">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D95">
         <v>3870</v>
@@ -2476,16 +2962,22 @@
       <c r="E95">
         <v>2016</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95">
+        <v>4471262.193</v>
+      </c>
+      <c r="G95">
+        <v>443316.4678</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="1">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C96" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D96">
         <v>3145</v>
@@ -2493,16 +2985,22 @@
       <c r="E96">
         <v>2016</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96">
+        <v>4470671.33</v>
+      </c>
+      <c r="G96">
+        <v>444074.8694</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="1">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D97">
         <v>3734</v>
@@ -2510,16 +3008,22 @@
       <c r="E97">
         <v>2016</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97">
+        <v>4470708.716</v>
+      </c>
+      <c r="G97">
+        <v>445907.486</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="1">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D98">
         <v>2598</v>
@@ -2527,16 +3031,22 @@
       <c r="E98">
         <v>2016</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98">
+        <v>4471314.521</v>
+      </c>
+      <c r="G98">
+        <v>444982.7317</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" s="1">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C99" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D99">
         <v>4308</v>
@@ -2544,16 +3054,22 @@
       <c r="E99">
         <v>2016</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99">
+        <v>4472306.995</v>
+      </c>
+      <c r="G99">
+        <v>444116.7652</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" s="1">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C100" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D100">
         <v>5953</v>
@@ -2562,15 +3078,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:7">
       <c r="A101" s="1">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D101">
         <v>634</v>
@@ -2578,16 +3094,22 @@
       <c r="E101">
         <v>2016</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101">
+        <v>4472183.36</v>
+      </c>
+      <c r="G101">
+        <v>446353.3523</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D102">
         <v>409</v>
@@ -2595,16 +3117,22 @@
       <c r="E102">
         <v>2016</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102">
+        <v>4473295.298</v>
+      </c>
+      <c r="G102">
+        <v>446804.3855</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" s="1">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D103">
         <v>1513</v>
@@ -2612,16 +3140,22 @@
       <c r="E103">
         <v>2016</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103">
+        <v>4473543.376</v>
+      </c>
+      <c r="G103">
+        <v>445646.4672</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" s="1">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C104" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D104">
         <v>1183</v>
@@ -2629,16 +3163,22 @@
       <c r="E104">
         <v>2016</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104">
+        <v>4473682.217</v>
+      </c>
+      <c r="G104">
+        <v>444272.189</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="1">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D105">
         <v>1181</v>
@@ -2646,16 +3186,22 @@
       <c r="E105">
         <v>2016</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105">
+        <v>4472512.703</v>
+      </c>
+      <c r="G105">
+        <v>445115.9638</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" s="1">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D106">
         <v>940</v>
@@ -2663,16 +3209,22 @@
       <c r="E106">
         <v>2016</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106">
+        <v>4472936.191</v>
+      </c>
+      <c r="G106">
+        <v>445482.8128</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" s="1">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C107" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D107">
         <v>12867</v>
@@ -2681,15 +3233,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:7">
       <c r="A108" s="1">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C108" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D108">
         <v>3125</v>
@@ -2697,16 +3249,22 @@
       <c r="E108">
         <v>2016</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108">
+        <v>4474850.803</v>
+      </c>
+      <c r="G108">
+        <v>445079.4926</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" s="1">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C109" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D109">
         <v>4015</v>
@@ -2714,16 +3272,22 @@
       <c r="E109">
         <v>2016</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109">
+        <v>4475266.901</v>
+      </c>
+      <c r="G109">
+        <v>446095.6831</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110" s="1">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D110">
         <v>1626</v>
@@ -2731,16 +3295,22 @@
       <c r="E110">
         <v>2016</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110">
+        <v>4476462.964</v>
+      </c>
+      <c r="G110">
+        <v>445289.7605</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" s="1">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C111" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D111">
         <v>1185</v>
@@ -2748,16 +3318,22 @@
       <c r="E111">
         <v>2016</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111">
+        <v>4476721.345</v>
+      </c>
+      <c r="G111">
+        <v>444934.1577</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112" s="1">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D112">
         <v>959</v>
@@ -2765,16 +3341,22 @@
       <c r="E112">
         <v>2016</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112">
+        <v>4477117.637</v>
+      </c>
+      <c r="G112">
+        <v>444582.4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" s="1">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C113" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D113">
         <v>524</v>
@@ -2782,16 +3364,22 @@
       <c r="E113">
         <v>2016</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113">
+        <v>4477988.461</v>
+      </c>
+      <c r="G113">
+        <v>444343.151</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114" s="1">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D114">
         <v>254</v>
@@ -2799,16 +3387,22 @@
       <c r="E114">
         <v>2016</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114">
+        <v>4478807.34</v>
+      </c>
+      <c r="G114">
+        <v>444014.4325</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115" s="1">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C115" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D115">
         <v>47</v>
@@ -2816,16 +3410,22 @@
       <c r="E115">
         <v>2016</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115">
+        <v>4479501.192</v>
+      </c>
+      <c r="G115">
+        <v>443626.7881</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116" s="1">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D116">
         <v>856</v>
@@ -2833,16 +3433,22 @@
       <c r="E116">
         <v>2016</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116">
+        <v>4480877.84</v>
+      </c>
+      <c r="G116">
+        <v>443334.1197</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" s="1">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D117">
         <v>9178</v>
@@ -2851,15 +3457,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:7">
       <c r="A118" s="1">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C118" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D118">
         <v>209</v>
@@ -2867,16 +3473,22 @@
       <c r="E118">
         <v>2016</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118">
+        <v>4478175.942</v>
+      </c>
+      <c r="G118">
+        <v>447754.9382</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" s="1">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D119">
         <v>417</v>
@@ -2884,16 +3496,22 @@
       <c r="E119">
         <v>2016</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119">
+        <v>4478532.529</v>
+      </c>
+      <c r="G119">
+        <v>446151.4886</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120" s="1">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D120">
         <v>2009</v>
@@ -2901,16 +3519,22 @@
       <c r="E120">
         <v>2016</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120">
+        <v>4479433.42</v>
+      </c>
+      <c r="G120">
+        <v>445426.2189</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121" s="1">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C121" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D121">
         <v>3257</v>
@@ -2918,16 +3542,22 @@
       <c r="E121">
         <v>2016</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121">
+        <v>4480401.898</v>
+      </c>
+      <c r="G121">
+        <v>445152.0269</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122" s="1">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D122">
         <v>1025</v>
@@ -2935,16 +3565,22 @@
       <c r="E122">
         <v>2016</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122">
+        <v>4480844.351</v>
+      </c>
+      <c r="G122">
+        <v>444105.2521</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123" s="1">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D123">
         <v>2013</v>
@@ -2952,16 +3588,22 @@
       <c r="E123">
         <v>2016</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123">
+        <v>4482753.289</v>
+      </c>
+      <c r="G123">
+        <v>446176.0779</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
       <c r="A124" s="1">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D124">
         <v>12533</v>
@@ -2970,15 +3612,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:7">
       <c r="A125" s="1">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C125" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D125">
         <v>4245</v>
@@ -2987,15 +3629,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:7">
       <c r="A126" s="1">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D126">
         <v>1751</v>
@@ -3003,16 +3645,22 @@
       <c r="E126">
         <v>2016</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126">
+        <v>4465820.907</v>
+      </c>
+      <c r="G126">
+        <v>441533.8022</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127" s="1">
-        <v>3</v>
+        <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D127">
         <v>1136</v>
@@ -3020,16 +3668,22 @@
       <c r="E127">
         <v>2016</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127">
+        <v>4465394.096</v>
+      </c>
+      <c r="G127">
+        <v>442559.7779</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128" s="1">
-        <v>4</v>
+        <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D128">
         <v>2973</v>
@@ -3037,16 +3691,22 @@
       <c r="E128">
         <v>2016</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128">
+        <v>4467464.76</v>
+      </c>
+      <c r="G128">
+        <v>441536.5956</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
       <c r="A129" s="1">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C129" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D129">
         <v>2248</v>
@@ -3054,44 +3714,50 @@
       <c r="E129">
         <v>2016</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129">
+        <v>4467482.211</v>
+      </c>
+      <c r="G129">
+        <v>440632.5318</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
       <c r="A130" s="1">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E130">
         <v>2016</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:7">
       <c r="A131" s="1">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E131">
         <v>2016</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:7">
       <c r="A132" s="1">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D132">
         <v>7982</v>
@@ -3100,15 +3766,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:7">
       <c r="A133" s="1">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D133">
         <v>6180</v>
@@ -3116,16 +3782,22 @@
       <c r="E133">
         <v>2016</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133">
+        <v>4466332.267</v>
+      </c>
+      <c r="G133">
+        <v>447496.1334</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
       <c r="A134" s="1">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D134">
         <v>1734</v>
@@ -3133,86 +3805,92 @@
       <c r="E134">
         <v>2016</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134">
+        <v>4470494.392</v>
+      </c>
+      <c r="G134">
+        <v>448110.1432</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
       <c r="A135" s="1">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C135" t="s">
+        <v>140</v>
+      </c>
+      <c r="E135">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136" t="s">
+        <v>141</v>
+      </c>
+      <c r="E136">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137" t="s">
+        <v>142</v>
+      </c>
+      <c r="E137">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" t="s">
+        <v>135</v>
+      </c>
+      <c r="E138">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" t="s">
+        <v>136</v>
+      </c>
+      <c r="E139">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="E135">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="1">
-        <v>4</v>
-      </c>
-      <c r="B136" t="s">
-        <v>4</v>
-      </c>
-      <c r="C136" t="s">
-        <v>139</v>
-      </c>
-      <c r="E136">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="1">
-        <v>5</v>
-      </c>
-      <c r="B137" t="s">
-        <v>4</v>
-      </c>
-      <c r="C137" t="s">
-        <v>140</v>
-      </c>
-      <c r="E137">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
-      <c r="A138" s="1">
-        <v>6</v>
-      </c>
-      <c r="B138" t="s">
-        <v>4</v>
-      </c>
-      <c r="C138" t="s">
-        <v>133</v>
-      </c>
-      <c r="E138">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="1">
-        <v>7</v>
-      </c>
-      <c r="B139" t="s">
-        <v>4</v>
-      </c>
-      <c r="C139" t="s">
-        <v>134</v>
-      </c>
-      <c r="E139">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="1">
-        <v>0</v>
-      </c>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D140">
         <v>5144</v>
@@ -3221,15 +3899,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:7">
       <c r="A141" s="1">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D141">
         <v>3475</v>
@@ -3237,16 +3915,22 @@
       <c r="E141">
         <v>2016</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141">
+        <v>4471000.988</v>
+      </c>
+      <c r="G141">
+        <v>450789.392</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
       <c r="A142" s="1">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D142">
         <v>1591</v>
@@ -3255,85 +3939,85 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:7">
       <c r="A143" s="1">
-        <v>3</v>
+        <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E143">
         <v>2016</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:7">
       <c r="A144" s="1">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E144">
         <v>2016</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:7">
       <c r="A145" s="1">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E145">
         <v>2016</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:7">
       <c r="A146" s="1">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C146" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E146">
         <v>2016</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:7">
       <c r="A147" s="1">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E147">
         <v>2016</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:7">
       <c r="A148" s="1">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D148">
         <v>10595</v>
@@ -3342,15 +4026,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:7">
       <c r="A149" s="1">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C149" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D149">
         <v>1987</v>
@@ -3358,16 +4042,22 @@
       <c r="E149">
         <v>2016</v>
       </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="F149">
+        <v>4476263.737</v>
+      </c>
+      <c r="G149">
+        <v>446981.6721</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
       <c r="A150" s="1">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D150">
         <v>833</v>
@@ -3375,16 +4065,22 @@
       <c r="E150">
         <v>2016</v>
       </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="F150">
+        <v>4475772.544</v>
+      </c>
+      <c r="G150">
+        <v>447680.4837</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
       <c r="A151" s="1">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D151">
         <v>853</v>
@@ -3392,16 +4088,22 @@
       <c r="E151">
         <v>2016</v>
       </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="F151">
+        <v>4475241.334</v>
+      </c>
+      <c r="G151">
+        <v>447234.3454</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
       <c r="A152" s="1">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D152">
         <v>1911</v>
@@ -3409,16 +4111,22 @@
       <c r="E152">
         <v>2016</v>
       </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="F152">
+        <v>4474693.643</v>
+      </c>
+      <c r="G152">
+        <v>447607.4973</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
       <c r="A153" s="1">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D153">
         <v>1501</v>
@@ -3426,16 +4134,22 @@
       <c r="E153">
         <v>2016</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153">
+        <v>4475395.532</v>
+      </c>
+      <c r="G153">
+        <v>449590.4285</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
       <c r="A154" s="1">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D154">
         <v>791</v>
@@ -3443,16 +4157,22 @@
       <c r="E154">
         <v>2016</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154">
+        <v>4477317.169</v>
+      </c>
+      <c r="G154">
+        <v>451648.3991</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
       <c r="A155" s="1">
-        <v>7</v>
+        <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D155">
         <v>2001</v>
@@ -3460,16 +4180,22 @@
       <c r="E155">
         <v>2016</v>
       </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="F155">
+        <v>4477135.693</v>
+      </c>
+      <c r="G155">
+        <v>448224.083</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
       <c r="A156" s="1">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D156">
         <v>530</v>
@@ -3477,16 +4203,22 @@
       <c r="E156">
         <v>2016</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156">
+        <v>4477373.192</v>
+      </c>
+      <c r="G156">
+        <v>446491.5939</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
       <c r="A157" s="1">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D157">
         <v>2241</v>
@@ -3495,15 +4227,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:7">
       <c r="A158" s="1">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D158">
         <v>751</v>
@@ -3511,16 +4243,22 @@
       <c r="E158">
         <v>2016</v>
       </c>
-    </row>
-    <row r="159" spans="1:5">
+      <c r="F158">
+        <v>4478581.448</v>
+      </c>
+      <c r="G158">
+        <v>449818.2184</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
       <c r="A159" s="1">
-        <v>2</v>
+        <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D159">
         <v>140</v>
@@ -3528,16 +4266,22 @@
       <c r="E159">
         <v>2016</v>
       </c>
-    </row>
-    <row r="160" spans="1:5">
+      <c r="F159">
+        <v>4481029.075</v>
+      </c>
+      <c r="G159">
+        <v>452237.8537</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
       <c r="A160" s="1">
-        <v>3</v>
+        <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D160">
         <v>539</v>
@@ -3545,16 +4289,22 @@
       <c r="E160">
         <v>2016</v>
       </c>
-    </row>
-    <row r="161" spans="1:5">
+      <c r="F160">
+        <v>4480530.185</v>
+      </c>
+      <c r="G160">
+        <v>450931.3676</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
       <c r="A161" s="1">
-        <v>4</v>
+        <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D161">
         <v>531</v>
@@ -3562,22 +4312,34 @@
       <c r="E161">
         <v>2016</v>
       </c>
-    </row>
-    <row r="162" spans="1:5">
+      <c r="F161">
+        <v>4480810.557</v>
+      </c>
+      <c r="G161">
+        <v>448842.3002</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
       <c r="A162" s="1">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C162" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D162">
         <v>232</v>
       </c>
       <c r="E162">
         <v>2016</v>
+      </c>
+      <c r="F162">
+        <v>4479457.295</v>
+      </c>
+      <c r="G162">
+        <v>448527.2781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>